<commit_message>
Update word schema composite pk)
</commit_message>
<xml_diff>
--- a/app/Vocab_list .xlsx
+++ b/app/Vocab_list .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0\Desktop\COMP3901-Capstone\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E8B822-C0B8-43F7-8E49-791C7F1B7846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0517D8-EE5E-42E9-97E7-9B7A70B74567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22260" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22260" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Words" sheetId="1" r:id="rId1"/>
@@ -4248,8 +4248,8 @@
   </sheetPr>
   <dimension ref="A1:AA955"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4321,10 +4321,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>377</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -4334,6 +4334,9 @@
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>11</v>
@@ -37642,13 +37645,13 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>